<commit_message>
updates the gantt chart
</commit_message>
<xml_diff>
--- a/source/prodrive_gantt_chart.xlsx
+++ b/source/prodrive_gantt_chart.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\flashdisk\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
@@ -133,7 +128,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -246,18 +241,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -265,40 +254,55 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -359,7 +363,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -394,7 +398,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -571,7 +575,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -585,7 +589,7 @@
       <pane xSplit="10" ySplit="8" topLeftCell="K9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AJ10" sqref="AJ10"/>
+      <selection pane="bottomRight" activeCell="AD26" sqref="AD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,314 +598,315 @@
     <col min="2" max="2" width="25.28515625" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="10" width="5.7109375" customWidth="1"/>
     <col min="11" max="16" width="4.28515625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.28515625" style="10" customWidth="1"/>
+    <col min="17" max="17" width="4.28515625" style="7" customWidth="1"/>
     <col min="18" max="23" width="4.28515625" style="1" customWidth="1"/>
-    <col min="24" max="24" width="4.28515625" style="10" customWidth="1"/>
-    <col min="25" max="25" width="4.28515625" style="17" customWidth="1"/>
-    <col min="26" max="30" width="4.28515625" style="1" customWidth="1"/>
-    <col min="31" max="31" width="4.28515625" style="10" customWidth="1"/>
+    <col min="24" max="24" width="4.28515625" style="7" customWidth="1"/>
+    <col min="25" max="25" width="4.28515625" style="10" customWidth="1"/>
+    <col min="26" max="26" width="4.28515625" style="12" customWidth="1"/>
+    <col min="27" max="30" width="4.28515625" style="1" customWidth="1"/>
+    <col min="31" max="31" width="4.28515625" style="7" customWidth="1"/>
     <col min="32" max="37" width="4.28515625" style="1" customWidth="1"/>
-    <col min="38" max="38" width="4.28515625" style="10" customWidth="1"/>
+    <col min="38" max="38" width="4.28515625" style="7" customWidth="1"/>
     <col min="39" max="44" width="4.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:45" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="Y1" s="16"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="Z1" s="11"/>
     </row>
     <row r="2" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
     </row>
     <row r="3" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="19"/>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="13"/>
       <c r="D3" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
     </row>
     <row r="4" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="12"/>
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="8"/>
       <c r="D4" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
     </row>
     <row r="5" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="C5" s="22"/>
+      <c r="C5" s="15"/>
       <c r="D5" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
     </row>
     <row r="6" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="C6" s="20"/>
+      <c r="C6" s="14"/>
       <c r="D6" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="2" t="s">
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="R6" s="2" t="s">
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+      <c r="R6" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
-      <c r="U6" s="2"/>
-      <c r="V6" s="2"/>
-      <c r="W6" s="2"/>
-      <c r="Y6" s="15" t="s">
+      <c r="S6" s="17"/>
+      <c r="T6" s="17"/>
+      <c r="U6" s="17"/>
+      <c r="V6" s="17"/>
+      <c r="W6" s="17"/>
+      <c r="Y6" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="Z6" s="15"/>
-      <c r="AA6" s="15"/>
-      <c r="AB6" s="15"/>
-      <c r="AC6" s="15"/>
-      <c r="AD6" s="15"/>
-      <c r="AF6" s="2" t="s">
+      <c r="Z6" s="18"/>
+      <c r="AA6" s="18"/>
+      <c r="AB6" s="18"/>
+      <c r="AC6" s="18"/>
+      <c r="AD6" s="18"/>
+      <c r="AF6" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="AG6" s="2"/>
-      <c r="AH6" s="2"/>
-      <c r="AI6" s="2"/>
-      <c r="AJ6" s="2"/>
-      <c r="AK6" s="2"/>
-      <c r="AM6" s="2" t="s">
+      <c r="AG6" s="17"/>
+      <c r="AH6" s="17"/>
+      <c r="AI6" s="17"/>
+      <c r="AJ6" s="17"/>
+      <c r="AK6" s="17"/>
+      <c r="AM6" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="AN6" s="2"/>
-      <c r="AO6" s="2"/>
-      <c r="AP6" s="2"/>
-      <c r="AQ6" s="2"/>
-      <c r="AR6" s="2"/>
+      <c r="AN6" s="17"/>
+      <c r="AO6" s="17"/>
+      <c r="AP6" s="17"/>
+      <c r="AQ6" s="17"/>
+      <c r="AR6" s="17"/>
     </row>
     <row r="7" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="H7" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="I7" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="14" t="s">
+      <c r="J7" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="K7" s="8">
+      <c r="K7" s="16">
         <v>41372</v>
       </c>
-      <c r="L7" s="8">
+      <c r="L7" s="16">
         <v>41373</v>
       </c>
-      <c r="M7" s="8">
+      <c r="M7" s="16">
         <v>41374</v>
       </c>
-      <c r="N7" s="8">
+      <c r="N7" s="16">
         <v>41375</v>
       </c>
-      <c r="O7" s="8">
+      <c r="O7" s="16">
         <v>41376</v>
       </c>
-      <c r="P7" s="8">
+      <c r="P7" s="16">
         <v>41377</v>
       </c>
-      <c r="Q7" s="11">
+      <c r="Q7" s="19">
         <v>41378</v>
       </c>
-      <c r="R7" s="8">
+      <c r="R7" s="16">
         <v>41379</v>
       </c>
-      <c r="S7" s="8">
+      <c r="S7" s="16">
         <v>41380</v>
       </c>
-      <c r="T7" s="8">
+      <c r="T7" s="16">
         <v>41381</v>
       </c>
-      <c r="U7" s="8">
+      <c r="U7" s="16">
         <v>41382</v>
       </c>
-      <c r="V7" s="8">
+      <c r="V7" s="16">
         <v>41383</v>
       </c>
-      <c r="W7" s="8">
+      <c r="W7" s="16">
         <v>41384</v>
       </c>
-      <c r="X7" s="11">
+      <c r="X7" s="19">
         <v>41385</v>
       </c>
-      <c r="Y7" s="18">
+      <c r="Y7" s="23">
         <v>41386</v>
       </c>
-      <c r="Z7" s="8">
+      <c r="Z7" s="20">
         <v>41387</v>
       </c>
-      <c r="AA7" s="8">
+      <c r="AA7" s="16">
         <v>41388</v>
       </c>
-      <c r="AB7" s="8">
+      <c r="AB7" s="16">
         <v>41389</v>
       </c>
-      <c r="AC7" s="8">
+      <c r="AC7" s="16">
         <v>41390</v>
       </c>
-      <c r="AD7" s="8">
+      <c r="AD7" s="16">
         <v>41391</v>
       </c>
-      <c r="AE7" s="11">
+      <c r="AE7" s="19">
         <v>41392</v>
       </c>
-      <c r="AF7" s="8">
+      <c r="AF7" s="16">
         <v>41393</v>
       </c>
-      <c r="AG7" s="8">
+      <c r="AG7" s="16">
         <v>41394</v>
       </c>
-      <c r="AH7" s="8">
+      <c r="AH7" s="16">
         <v>41395</v>
       </c>
-      <c r="AI7" s="8">
+      <c r="AI7" s="16">
         <v>41396</v>
       </c>
-      <c r="AJ7" s="8">
+      <c r="AJ7" s="16">
         <v>41397</v>
       </c>
-      <c r="AK7" s="8">
+      <c r="AK7" s="16">
         <v>41398</v>
       </c>
-      <c r="AL7" s="11">
+      <c r="AL7" s="19">
         <v>41399</v>
       </c>
-      <c r="AM7" s="8">
+      <c r="AM7" s="16">
         <v>41400</v>
       </c>
-      <c r="AN7" s="8">
+      <c r="AN7" s="16">
         <v>41401</v>
       </c>
-      <c r="AO7" s="8">
+      <c r="AO7" s="16">
         <v>41402</v>
       </c>
-      <c r="AP7" s="8">
+      <c r="AP7" s="16">
         <v>41403</v>
       </c>
-      <c r="AQ7" s="8">
+      <c r="AQ7" s="16">
         <v>41404</v>
       </c>
-      <c r="AR7" s="8">
+      <c r="AR7" s="16">
         <v>41405</v>
       </c>
     </row>
     <row r="8" spans="1:45" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="11"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="8"/>
-      <c r="T8" s="8"/>
-      <c r="U8" s="8"/>
-      <c r="V8" s="8"/>
-      <c r="W8" s="8"/>
-      <c r="X8" s="11"/>
-      <c r="Y8" s="18"/>
-      <c r="Z8" s="8"/>
-      <c r="AA8" s="8"/>
-      <c r="AB8" s="8"/>
-      <c r="AC8" s="8"/>
-      <c r="AD8" s="8"/>
-      <c r="AE8" s="11"/>
-      <c r="AF8" s="8"/>
-      <c r="AG8" s="8"/>
-      <c r="AH8" s="8"/>
-      <c r="AI8" s="8"/>
-      <c r="AJ8" s="8"/>
-      <c r="AK8" s="8"/>
-      <c r="AL8" s="11"/>
-      <c r="AM8" s="8"/>
-      <c r="AN8" s="8"/>
-      <c r="AO8" s="8"/>
-      <c r="AP8" s="8"/>
-      <c r="AQ8" s="8"/>
-      <c r="AR8" s="8"/>
-      <c r="AS8" s="7"/>
+      <c r="A8" s="22"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="19"/>
+      <c r="R8" s="16"/>
+      <c r="S8" s="16"/>
+      <c r="T8" s="16"/>
+      <c r="U8" s="16"/>
+      <c r="V8" s="16"/>
+      <c r="W8" s="16"/>
+      <c r="X8" s="19"/>
+      <c r="Y8" s="23"/>
+      <c r="Z8" s="20"/>
+      <c r="AA8" s="16"/>
+      <c r="AB8" s="16"/>
+      <c r="AC8" s="16"/>
+      <c r="AD8" s="16"/>
+      <c r="AE8" s="19"/>
+      <c r="AF8" s="16"/>
+      <c r="AG8" s="16"/>
+      <c r="AH8" s="16"/>
+      <c r="AI8" s="16"/>
+      <c r="AJ8" s="16"/>
+      <c r="AK8" s="16"/>
+      <c r="AL8" s="19"/>
+      <c r="AM8" s="16"/>
+      <c r="AN8" s="16"/>
+      <c r="AO8" s="16"/>
+      <c r="AP8" s="16"/>
+      <c r="AQ8" s="16"/>
+      <c r="AR8" s="16"/>
+      <c r="AS8" s="5"/>
     </row>
     <row r="9" spans="1:45" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+      <c r="A9" s="3">
         <v>1</v>
       </c>
       <c r="B9" t="s">
@@ -910,34 +915,34 @@
       <c r="C9" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="4">
         <v>41372</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="4">
         <v>41393</v>
       </c>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="12"/>
-      <c r="R9" s="12"/>
-      <c r="S9" s="12"/>
-      <c r="T9" s="12"/>
-      <c r="U9" s="12"/>
-      <c r="V9" s="12"/>
-      <c r="W9" s="12"/>
-      <c r="Y9" s="23"/>
-      <c r="Z9" s="9"/>
-      <c r="AA9" s="9"/>
-      <c r="AB9" s="9"/>
-      <c r="AC9" s="9"/>
-      <c r="AD9" s="9"/>
-      <c r="AF9" s="9"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="8"/>
+      <c r="U9" s="8"/>
+      <c r="V9" s="8"/>
+      <c r="W9" s="8"/>
+      <c r="Y9" s="24"/>
+      <c r="Z9" s="25"/>
+      <c r="AA9" s="6"/>
+      <c r="AB9" s="6"/>
+      <c r="AC9" s="6"/>
+      <c r="AD9" s="6"/>
+      <c r="AF9" s="6"/>
     </row>
     <row r="10" spans="1:45" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+      <c r="A10" s="3">
         <v>1.1000000000000001</v>
       </c>
       <c r="B10" t="s">
@@ -946,34 +951,34 @@
       <c r="C10" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="4">
         <v>41372</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="4">
         <v>41393</v>
       </c>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="12"/>
-      <c r="R10" s="12"/>
-      <c r="S10" s="12"/>
-      <c r="T10" s="12"/>
-      <c r="U10" s="12"/>
-      <c r="V10" s="12"/>
-      <c r="W10" s="12"/>
-      <c r="Y10" s="23"/>
-      <c r="Z10" s="9"/>
-      <c r="AA10" s="9"/>
-      <c r="AB10" s="9"/>
-      <c r="AC10" s="9"/>
-      <c r="AD10" s="9"/>
-      <c r="AF10" s="9"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="8"/>
+      <c r="T10" s="8"/>
+      <c r="U10" s="8"/>
+      <c r="V10" s="8"/>
+      <c r="W10" s="8"/>
+      <c r="Y10" s="24"/>
+      <c r="Z10" s="25"/>
+      <c r="AA10" s="6"/>
+      <c r="AB10" s="6"/>
+      <c r="AC10" s="6"/>
+      <c r="AD10" s="6"/>
+      <c r="AF10" s="6"/>
     </row>
     <row r="11" spans="1:45" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+      <c r="A11" s="3">
         <v>2</v>
       </c>
       <c r="B11" t="s">
@@ -982,34 +987,34 @@
       <c r="C11" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="4">
         <v>41372</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="4">
         <v>41393</v>
       </c>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
-      <c r="O11" s="12"/>
-      <c r="P11" s="12"/>
-      <c r="R11" s="12"/>
-      <c r="S11" s="12"/>
-      <c r="T11" s="12"/>
-      <c r="U11" s="12"/>
-      <c r="V11" s="12"/>
-      <c r="W11" s="12"/>
-      <c r="Y11" s="23"/>
-      <c r="Z11" s="9"/>
-      <c r="AA11" s="9"/>
-      <c r="AB11" s="9"/>
-      <c r="AC11" s="9"/>
-      <c r="AD11" s="9"/>
-      <c r="AF11" s="9"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="8"/>
+      <c r="T11" s="8"/>
+      <c r="U11" s="8"/>
+      <c r="V11" s="8"/>
+      <c r="W11" s="8"/>
+      <c r="Y11" s="24"/>
+      <c r="Z11" s="25"/>
+      <c r="AA11" s="6"/>
+      <c r="AB11" s="6"/>
+      <c r="AC11" s="6"/>
+      <c r="AD11" s="6"/>
+      <c r="AF11" s="6"/>
     </row>
     <row r="12" spans="1:45" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+      <c r="A12" s="3">
         <v>2.1</v>
       </c>
       <c r="B12" t="s">
@@ -1018,39 +1023,39 @@
       <c r="C12" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="4">
         <v>41372</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="4">
         <v>41398</v>
       </c>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
-      <c r="O12" s="12"/>
-      <c r="P12" s="12"/>
-      <c r="R12" s="12"/>
-      <c r="S12" s="12"/>
-      <c r="T12" s="12"/>
-      <c r="U12" s="12"/>
-      <c r="V12" s="12"/>
-      <c r="W12" s="12"/>
-      <c r="Y12" s="23"/>
-      <c r="Z12" s="9"/>
-      <c r="AA12" s="9"/>
-      <c r="AB12" s="9"/>
-      <c r="AC12" s="9"/>
-      <c r="AD12" s="9"/>
-      <c r="AF12" s="9"/>
-      <c r="AG12" s="9"/>
-      <c r="AH12" s="9"/>
-      <c r="AI12" s="9"/>
-      <c r="AJ12" s="9"/>
-      <c r="AK12" s="9"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="8"/>
+      <c r="T12" s="8"/>
+      <c r="U12" s="8"/>
+      <c r="V12" s="8"/>
+      <c r="W12" s="8"/>
+      <c r="Y12" s="24"/>
+      <c r="Z12" s="25"/>
+      <c r="AA12" s="6"/>
+      <c r="AB12" s="6"/>
+      <c r="AC12" s="6"/>
+      <c r="AD12" s="6"/>
+      <c r="AF12" s="6"/>
+      <c r="AG12" s="6"/>
+      <c r="AH12" s="6"/>
+      <c r="AI12" s="6"/>
+      <c r="AJ12" s="6"/>
+      <c r="AK12" s="6"/>
     </row>
     <row r="13" spans="1:45" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
+      <c r="A13" s="3">
         <v>3</v>
       </c>
       <c r="B13" t="s">
@@ -1059,16 +1064,16 @@
       <c r="C13" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="4">
         <v>41387</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="4">
         <v>41387</v>
       </c>
-      <c r="Z13" s="21"/>
+      <c r="Z13" s="26"/>
     </row>
     <row r="14" spans="1:45" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+      <c r="A14" s="3">
         <v>4</v>
       </c>
       <c r="B14" t="s">
@@ -1077,21 +1082,21 @@
       <c r="C14" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="4">
         <v>41393</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="4">
         <v>41398</v>
       </c>
-      <c r="AF14" s="9"/>
-      <c r="AG14" s="9"/>
-      <c r="AH14" s="9"/>
-      <c r="AI14" s="9"/>
-      <c r="AJ14" s="9"/>
-      <c r="AK14" s="9"/>
+      <c r="AF14" s="6"/>
+      <c r="AG14" s="6"/>
+      <c r="AH14" s="6"/>
+      <c r="AI14" s="6"/>
+      <c r="AJ14" s="6"/>
+      <c r="AK14" s="6"/>
     </row>
     <row r="15" spans="1:45" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
+      <c r="A15" s="3">
         <v>4.0999999999999996</v>
       </c>
       <c r="B15" t="s">
@@ -1100,20 +1105,20 @@
       <c r="C15" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="4">
         <v>41387</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="4">
         <v>41391</v>
       </c>
-      <c r="Z15" s="9"/>
-      <c r="AA15" s="9"/>
-      <c r="AB15" s="9"/>
-      <c r="AC15" s="9"/>
-      <c r="AD15" s="9"/>
+      <c r="Z15" s="25"/>
+      <c r="AA15" s="6"/>
+      <c r="AB15" s="6"/>
+      <c r="AC15" s="6"/>
+      <c r="AD15" s="6"/>
     </row>
     <row r="16" spans="1:45" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
+      <c r="A16" s="3">
         <v>5</v>
       </c>
       <c r="B16" t="s">
@@ -1122,13 +1127,13 @@
       <c r="C16" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="4">
         <v>41400</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="4">
         <v>41400</v>
       </c>
-      <c r="AM16" s="9"/>
+      <c r="AM16" s="6"/>
       <c r="AN16"/>
       <c r="AO16"/>
       <c r="AP16"/>
@@ -1136,7 +1141,7 @@
       <c r="AR16"/>
     </row>
     <row r="17" spans="1:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
+      <c r="A17" s="3">
         <v>6</v>
       </c>
       <c r="B17" t="s">
@@ -1145,21 +1150,21 @@
       <c r="C17" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="4">
         <v>41400</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="4">
         <v>41401</v>
       </c>
-      <c r="AM17" s="9"/>
-      <c r="AN17" s="9"/>
+      <c r="AM17" s="6"/>
+      <c r="AN17" s="6"/>
       <c r="AO17"/>
       <c r="AP17"/>
       <c r="AQ17"/>
       <c r="AR17"/>
     </row>
     <row r="18" spans="1:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
+      <c r="A18" s="3">
         <v>7</v>
       </c>
       <c r="B18" t="s">
@@ -1168,21 +1173,21 @@
       <c r="C18" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="4">
         <v>41402</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="4">
         <v>41405</v>
       </c>
       <c r="AM18"/>
       <c r="AN18"/>
-      <c r="AO18" s="9"/>
-      <c r="AP18" s="9"/>
-      <c r="AQ18" s="9"/>
-      <c r="AR18" s="9"/>
+      <c r="AO18" s="6"/>
+      <c r="AP18" s="6"/>
+      <c r="AQ18" s="6"/>
+      <c r="AR18" s="6"/>
     </row>
     <row r="19" spans="1:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
+      <c r="A19" s="3">
         <v>8</v>
       </c>
       <c r="B19" t="s">
@@ -1191,69 +1196,69 @@
       <c r="C19" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="4">
         <v>41403</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="4">
         <v>41405</v>
       </c>
-      <c r="AP19" s="9"/>
-      <c r="AQ19" s="9"/>
-      <c r="AR19" s="9"/>
+      <c r="AP19" s="6"/>
+      <c r="AQ19" s="6"/>
+      <c r="AR19" s="6"/>
     </row>
     <row r="20" spans="1:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
+      <c r="A20" s="3"/>
     </row>
     <row r="21" spans="1:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
+      <c r="A21" s="3"/>
     </row>
     <row r="22" spans="1:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
+      <c r="A22" s="3"/>
     </row>
     <row r="23" spans="1:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
+      <c r="A23" s="3"/>
     </row>
     <row r="24" spans="1:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
+      <c r="A24" s="3"/>
     </row>
     <row r="25" spans="1:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
+      <c r="A25" s="3"/>
     </row>
     <row r="26" spans="1:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
+      <c r="A26" s="3"/>
     </row>
     <row r="27" spans="1:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
+      <c r="A27" s="3"/>
     </row>
     <row r="28" spans="1:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
+      <c r="A28" s="3"/>
     </row>
     <row r="29" spans="1:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
+      <c r="A29" s="3"/>
     </row>
     <row r="30" spans="1:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
+      <c r="A30" s="3"/>
     </row>
     <row r="31" spans="1:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
+      <c r="A31" s="3"/>
     </row>
     <row r="32" spans="1:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
+      <c r="A32" s="3"/>
     </row>
     <row r="33" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
+      <c r="A33" s="3"/>
     </row>
     <row r="34" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
+      <c r="A34" s="3"/>
     </row>
     <row r="35" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
+      <c r="A35" s="3"/>
     </row>
     <row r="36" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="5"/>
+      <c r="A36" s="3"/>
     </row>
     <row r="37" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
+      <c r="A37" s="3"/>
     </row>
     <row r="38" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="39" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1267,6 +1272,39 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="Z2ePrRReoODAvBuP/diQ78sXjyYNGcYG68q8FAiq1hniodZ5jVHuj4cXHi3/weP/GI2miQHKKa6t8OrY5wjGAA==" saltValue="Inye3QM/IHHjUJBn3JtuXA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0"/>
   <mergeCells count="49">
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="W7:W8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="P7:P8"/>
+    <mergeCell ref="Q7:Q8"/>
+    <mergeCell ref="R7:R8"/>
+    <mergeCell ref="S7:S8"/>
+    <mergeCell ref="T7:T8"/>
+    <mergeCell ref="U7:U8"/>
+    <mergeCell ref="V7:V8"/>
+    <mergeCell ref="AF7:AF8"/>
+    <mergeCell ref="AG7:AG8"/>
+    <mergeCell ref="AH7:AH8"/>
+    <mergeCell ref="AI7:AI8"/>
+    <mergeCell ref="X7:X8"/>
+    <mergeCell ref="Y7:Y8"/>
+    <mergeCell ref="Z7:Z8"/>
+    <mergeCell ref="AA7:AA8"/>
+    <mergeCell ref="AB7:AB8"/>
+    <mergeCell ref="AC7:AC8"/>
     <mergeCell ref="AP7:AP8"/>
     <mergeCell ref="AQ7:AQ8"/>
     <mergeCell ref="AR7:AR8"/>
@@ -1283,39 +1321,6 @@
     <mergeCell ref="AO7:AO8"/>
     <mergeCell ref="AD7:AD8"/>
     <mergeCell ref="AE7:AE8"/>
-    <mergeCell ref="AF7:AF8"/>
-    <mergeCell ref="AG7:AG8"/>
-    <mergeCell ref="AH7:AH8"/>
-    <mergeCell ref="AI7:AI8"/>
-    <mergeCell ref="X7:X8"/>
-    <mergeCell ref="Y7:Y8"/>
-    <mergeCell ref="Z7:Z8"/>
-    <mergeCell ref="AA7:AA8"/>
-    <mergeCell ref="AB7:AB8"/>
-    <mergeCell ref="AC7:AC8"/>
-    <mergeCell ref="R7:R8"/>
-    <mergeCell ref="S7:S8"/>
-    <mergeCell ref="T7:T8"/>
-    <mergeCell ref="U7:U8"/>
-    <mergeCell ref="V7:V8"/>
-    <mergeCell ref="W7:W8"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="P7:P8"/>
-    <mergeCell ref="Q7:Q8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
adds form element generator
</commit_message>
<xml_diff>
--- a/source/prodrive_gantt_chart.xlsx
+++ b/source/prodrive_gantt_chart.xlsx
@@ -309,7 +309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -387,11 +387,11 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
@@ -402,11 +402,14 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -694,7 +697,7 @@
       <pane xSplit="10" ySplit="8" topLeftCell="K13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="D21" sqref="D21:E21"/>
+      <selection pane="bottomRight" activeCell="R20" activeCellId="1" sqref="AB20 R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -790,76 +793,76 @@
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
-      <c r="K6" s="35" t="s">
+      <c r="K6" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="L6" s="35"/>
-      <c r="M6" s="35"/>
-      <c r="N6" s="35"/>
-      <c r="O6" s="35"/>
-      <c r="P6" s="35"/>
-      <c r="R6" s="35" t="s">
+      <c r="L6" s="40"/>
+      <c r="M6" s="40"/>
+      <c r="N6" s="40"/>
+      <c r="O6" s="40"/>
+      <c r="P6" s="40"/>
+      <c r="R6" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="S6" s="35"/>
-      <c r="T6" s="35"/>
-      <c r="U6" s="35"/>
-      <c r="V6" s="35"/>
-      <c r="W6" s="35"/>
-      <c r="Y6" s="36" t="s">
+      <c r="S6" s="40"/>
+      <c r="T6" s="40"/>
+      <c r="U6" s="40"/>
+      <c r="V6" s="40"/>
+      <c r="W6" s="40"/>
+      <c r="Y6" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="Z6" s="36"/>
-      <c r="AA6" s="36"/>
-      <c r="AB6" s="36"/>
-      <c r="AC6" s="36"/>
-      <c r="AD6" s="36"/>
-      <c r="AF6" s="35" t="s">
+      <c r="Z6" s="41"/>
+      <c r="AA6" s="41"/>
+      <c r="AB6" s="41"/>
+      <c r="AC6" s="41"/>
+      <c r="AD6" s="41"/>
+      <c r="AF6" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="AG6" s="35"/>
-      <c r="AH6" s="35"/>
-      <c r="AI6" s="35"/>
-      <c r="AJ6" s="35"/>
-      <c r="AK6" s="35"/>
-      <c r="AM6" s="35" t="s">
+      <c r="AG6" s="40"/>
+      <c r="AH6" s="40"/>
+      <c r="AI6" s="40"/>
+      <c r="AJ6" s="40"/>
+      <c r="AK6" s="40"/>
+      <c r="AM6" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="AN6" s="35"/>
-      <c r="AO6" s="35"/>
-      <c r="AP6" s="35"/>
-      <c r="AQ6" s="35"/>
-      <c r="AR6" s="35"/>
+      <c r="AN6" s="40"/>
+      <c r="AO6" s="40"/>
+      <c r="AP6" s="40"/>
+      <c r="AQ6" s="40"/>
+      <c r="AR6" s="40"/>
     </row>
     <row r="7" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="40" t="s">
+      <c r="C7" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="40" t="s">
+      <c r="D7" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="40" t="s">
+      <c r="E7" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="41" t="s">
+      <c r="F7" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="41" t="s">
+      <c r="G7" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="41" t="s">
+      <c r="H7" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="41" t="s">
+      <c r="I7" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="41" t="s">
+      <c r="J7" s="36" t="s">
         <v>9</v>
       </c>
       <c r="K7" s="34">
@@ -966,16 +969,16 @@
       </c>
     </row>
     <row r="8" spans="1:45" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="40"/>
-      <c r="B8" s="40"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
+      <c r="A8" s="35"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="36"/>
       <c r="K8" s="34"/>
       <c r="L8" s="34"/>
       <c r="M8" s="34"/>
@@ -1514,7 +1517,7 @@
       <c r="Y20" s="23"/>
       <c r="Z20" s="24"/>
       <c r="AA20" s="24"/>
-      <c r="AB20" s="6"/>
+      <c r="AB20" s="42"/>
       <c r="AC20" s="26"/>
       <c r="AD20" s="26"/>
       <c r="AF20" s="26"/>
@@ -1840,39 +1843,6 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0"/>
   <mergeCells count="49">
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="W7:W8"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="P7:P8"/>
-    <mergeCell ref="Q7:Q8"/>
-    <mergeCell ref="R7:R8"/>
-    <mergeCell ref="S7:S8"/>
-    <mergeCell ref="T7:T8"/>
-    <mergeCell ref="U7:U8"/>
-    <mergeCell ref="V7:V8"/>
-    <mergeCell ref="AF7:AF8"/>
-    <mergeCell ref="AG7:AG8"/>
-    <mergeCell ref="AH7:AH8"/>
-    <mergeCell ref="AI7:AI8"/>
-    <mergeCell ref="X7:X8"/>
-    <mergeCell ref="Y7:Y8"/>
-    <mergeCell ref="Z7:Z8"/>
-    <mergeCell ref="AA7:AA8"/>
-    <mergeCell ref="AB7:AB8"/>
-    <mergeCell ref="AC7:AC8"/>
     <mergeCell ref="AP7:AP8"/>
     <mergeCell ref="AQ7:AQ8"/>
     <mergeCell ref="AR7:AR8"/>
@@ -1889,6 +1859,39 @@
     <mergeCell ref="AO7:AO8"/>
     <mergeCell ref="AD7:AD8"/>
     <mergeCell ref="AE7:AE8"/>
+    <mergeCell ref="AF7:AF8"/>
+    <mergeCell ref="AG7:AG8"/>
+    <mergeCell ref="AH7:AH8"/>
+    <mergeCell ref="AI7:AI8"/>
+    <mergeCell ref="X7:X8"/>
+    <mergeCell ref="Y7:Y8"/>
+    <mergeCell ref="Z7:Z8"/>
+    <mergeCell ref="AA7:AA8"/>
+    <mergeCell ref="AB7:AB8"/>
+    <mergeCell ref="AC7:AC8"/>
+    <mergeCell ref="W7:W8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="P7:P8"/>
+    <mergeCell ref="Q7:Q8"/>
+    <mergeCell ref="R7:R8"/>
+    <mergeCell ref="S7:S8"/>
+    <mergeCell ref="T7:T8"/>
+    <mergeCell ref="U7:U8"/>
+    <mergeCell ref="V7:V8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>